<commit_message>
Adicionando projeto de pegar cotações via yahoo
</commit_message>
<xml_diff>
--- a/Aula4/Produtos Atualizados.xlsx
+++ b/Aula4/Produtos Atualizados.xlsx
@@ -67,25 +67,25 @@
     <t>Ouro</t>
   </si>
   <si>
-    <t>7472.99</t>
-  </si>
-  <si>
-    <t>58264.20</t>
-  </si>
-  <si>
-    <t>8166.90</t>
-  </si>
-  <si>
-    <t>7250.47</t>
-  </si>
-  <si>
-    <t>36900.66</t>
-  </si>
-  <si>
-    <t>5129.51</t>
-  </si>
-  <si>
-    <t>6998.67</t>
+    <t>7608.36</t>
+  </si>
+  <si>
+    <t>58826.70</t>
+  </si>
+  <si>
+    <t>8314.85</t>
+  </si>
+  <si>
+    <t>7381.82</t>
+  </si>
+  <si>
+    <t>37256.91</t>
+  </si>
+  <si>
+    <t>5222.43</t>
+  </si>
+  <si>
+    <t>7097.57</t>
   </si>
 </sst>
 </file>
@@ -483,10 +483,10 @@
         <v>14</v>
       </c>
       <c r="D2">
-        <v>5.337899999999999</v>
+        <v>5.4346</v>
       </c>
       <c r="E2">
-        <v>5337.846621</v>
+        <v>5434.545654</v>
       </c>
       <c r="F2">
         <v>1.4</v>
@@ -506,10 +506,10 @@
         <v>15</v>
       </c>
       <c r="D3">
-        <v>6.4738</v>
+        <v>6.5363</v>
       </c>
       <c r="E3">
-        <v>29132.1</v>
+        <v>29413.35</v>
       </c>
       <c r="F3">
         <v>2</v>
@@ -529,10 +529,10 @@
         <v>14</v>
       </c>
       <c r="D4">
-        <v>5.337899999999999</v>
+        <v>5.4346</v>
       </c>
       <c r="E4">
-        <v>4804.056621</v>
+        <v>4891.085654</v>
       </c>
       <c r="F4">
         <v>1.7</v>
@@ -552,10 +552,10 @@
         <v>14</v>
       </c>
       <c r="D5">
-        <v>5.337899999999999</v>
+        <v>5.4346</v>
       </c>
       <c r="E5">
-        <v>4264.982099999999</v>
+        <v>4342.2454</v>
       </c>
       <c r="F5">
         <v>1.7</v>
@@ -575,10 +575,10 @@
         <v>15</v>
       </c>
       <c r="D6">
-        <v>6.4738</v>
+        <v>6.5363</v>
       </c>
       <c r="E6">
-        <v>19421.4</v>
+        <v>19608.9</v>
       </c>
       <c r="F6">
         <v>1.9</v>
@@ -598,10 +598,10 @@
         <v>14</v>
       </c>
       <c r="D7">
-        <v>5.337899999999999</v>
+        <v>5.4346</v>
       </c>
       <c r="E7">
-        <v>2564.754192</v>
+        <v>2611.216608</v>
       </c>
       <c r="F7">
         <v>2</v>
@@ -621,10 +621,10 @@
         <v>16</v>
       </c>
       <c r="D8">
-        <v>304.29</v>
+        <v>308.59</v>
       </c>
       <c r="E8">
-        <v>6085.8</v>
+        <v>6171.799999999999</v>
       </c>
       <c r="F8">
         <v>1.15</v>

</xml_diff>